<commit_message>
Update variables with citations.xlsx
</commit_message>
<xml_diff>
--- a/variables with citations.xlsx
+++ b/variables with citations.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="19815" windowHeight="5070"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="19815" windowHeight="5070" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FD" sheetId="1" r:id="rId1"/>
     <sheet name="TD" sheetId="4" r:id="rId2"/>
     <sheet name="MD" sheetId="5" r:id="rId3"/>
     <sheet name="SD" sheetId="6" r:id="rId4"/>
+    <sheet name="Common Prediction Techniques" sheetId="7" r:id="rId5"/>
+    <sheet name="Result metrics" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc74869092" localSheetId="0">FD!$A$3</definedName>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="373">
   <si>
     <t>Variables Name</t>
   </si>
@@ -955,12 +957,210 @@
   <si>
     <t>Miscellaneous Information</t>
   </si>
+  <si>
+    <t>gated recurrent unit</t>
+  </si>
+  <si>
+    <t>GRU</t>
+  </si>
+  <si>
+    <t>artificial neural network</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>Multilayer perceptron</t>
+  </si>
+  <si>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Deep neural network</t>
+  </si>
+  <si>
+    <t>DNN</t>
+  </si>
+  <si>
+    <t>Principal component analysis</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>Support vector Regression</t>
+  </si>
+  <si>
+    <t>SVR</t>
+  </si>
+  <si>
+    <t>Support vector machine</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>recurrent neural network</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>random forest</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>long short term memory</t>
+  </si>
+  <si>
+    <t>LSTM</t>
+  </si>
+  <si>
+    <t>k-Nearest neighbor</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Deep multilayer perceptron</t>
+  </si>
+  <si>
+    <t>DMLP</t>
+  </si>
+  <si>
+    <t>Convolutional neural network</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>Capital asset pricing model</t>
+  </si>
+  <si>
+    <t>CAPM</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F1-score</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>APE</t>
+  </si>
+  <si>
+    <t>absolute percentage error</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>mean absolute error</t>
+  </si>
+  <si>
+    <t>MAPE</t>
+  </si>
+  <si>
+    <t>mean absolute percentage Error</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>Matthews correlation coefficient</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>mean square error</t>
+  </si>
+  <si>
+    <t>NMSE</t>
+  </si>
+  <si>
+    <t>normalized mean squared error</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>Profitability</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>coefficient of determination</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>root mean square error</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>correlation coefficient</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Sharpe ratio</t>
+  </si>
+  <si>
+    <t>ARV</t>
+  </si>
+  <si>
+    <t>average relative variance</t>
+  </si>
+  <si>
+    <t>MDD</t>
+  </si>
+  <si>
+    <t>maximum drawdown</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>Return rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abbreviation </t>
+  </si>
+  <si>
+    <t>Complete Name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,20 +1168,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -989,11 +1199,13 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1004,6 +1216,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1034,7 +1252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1049,43 +1267,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1300,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -39132,4 +39445,314 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A1" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A3" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A4" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A5" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="39" thickBot="1">
+      <c r="A6" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A7" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A8" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="39" thickBot="1">
+      <c r="A9" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="39" thickBot="1">
+      <c r="A10" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A11" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="39" thickBot="1">
+      <c r="A12" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="39" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="39" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="39" thickBot="1">
+      <c r="A15" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="39" thickBot="1">
+      <c r="A16" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="39" thickBot="1">
+      <c r="A17" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A1" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="39" thickBot="1">
+      <c r="A4" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="39" thickBot="1">
+      <c r="A5" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A6" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="39" thickBot="1">
+      <c r="A7" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="39" thickBot="1">
+      <c r="A8" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A9" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A10" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="51.75" thickBot="1">
+      <c r="A11" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="39" thickBot="1">
+      <c r="A12" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="39" thickBot="1">
+      <c r="A15" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A16" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A17" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>